<commit_message>
edit communication uart and edit file exel frame
</commit_message>
<xml_diff>
--- a/Frame.xlsx
+++ b/Frame.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>0x55</t>
   </si>
@@ -47,18 +47,12 @@
     <t>2byte</t>
   </si>
   <si>
-    <t>TAIL BYTE</t>
-  </si>
-  <si>
     <t>0xFF</t>
   </si>
   <si>
     <t>0x0000U</t>
   </si>
   <si>
-    <t>1 action</t>
-  </si>
-  <si>
     <t>0 check</t>
   </si>
   <si>
@@ -72,6 +66,18 @@
   </si>
   <si>
     <t>CRC8bit</t>
+  </si>
+  <si>
+    <t>END BYTE</t>
+  </si>
+  <si>
+    <t>DLEN = 5</t>
+  </si>
+  <si>
+    <t>DLEN = 3</t>
+  </si>
+  <si>
+    <t>1 control</t>
   </si>
 </sst>
 </file>
@@ -155,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -163,22 +169,25 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,34 +468,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="11"/>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="F1" s="13"/>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -502,79 +511,138 @@
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D4" s="3"/>
+      <c r="E4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="13"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
       <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D15" s="3"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D17" s="3"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="E7:F7"/>
+  <mergeCells count="10">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>